<commit_message>
Completed Multi Bill Payment and Linking & De Linking tasks.
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor Code - WEB
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-6220\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-71620\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Limit Management Done, Manage Schedule partial work
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/DebitRegistration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-8262020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-922020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,9 +165,6 @@
     <t>4028052000002718</t>
   </si>
   <si>
-    <t>mojizabidi98</t>
-  </si>
-  <si>
     <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL P where P.PARAMETER_NAME ='LOGIN_AND_T_PWRD_DESC_BEFORE_LOGIN'</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>681168</t>
+  </si>
+  <si>
+    <t>MOJIZABIDI98</t>
   </si>
 </sst>
 </file>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AB1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="130.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -641,10 +641,10 @@
         <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -661,13 +661,13 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
@@ -676,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>40</v>
@@ -685,7 +685,7 @@
         <v>13</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>17</v>
@@ -727,10 +727,10 @@
         <v>30</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>